<commit_message>
Added Grant's A2597 observations, archived in Oct 2018
</commit_message>
<xml_diff>
--- a/ACCEPT observations.xlsx
+++ b/ACCEPT observations.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\University\Year 5\Summer Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\ACCEPT_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="273">
   <si>
     <t>1E0657_56</t>
   </si>
@@ -777,9 +777,6 @@
     <t>includes 1938.78 ks of calibration</t>
   </si>
   <si>
-    <t>Grant has 474.27 ks of observations which will be archived in October for Abell 2597</t>
-  </si>
-  <si>
     <t>has 83.64 ks of offset observations</t>
   </si>
   <si>
@@ -822,9 +819,6 @@
     <t>has 165.81 ks of grating observations</t>
   </si>
   <si>
-    <t>966 total observations</t>
-  </si>
-  <si>
     <t>All Observations ( * denotes a calibration)</t>
   </si>
   <si>
@@ -841,6 +835,9 @@
   </si>
   <si>
     <t>has 93.58 ks of grating observations</t>
+  </si>
+  <si>
+    <t>977 total observations</t>
   </si>
 </sst>
 </file>
@@ -1353,7 +1350,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1374,20 +1371,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1400,21 +1409,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1740,66 +1734,66 @@
   <dimension ref="A1:AT255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="2"/>
-    <col min="9" max="9" width="25" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="38" width="9.140625" style="3" customWidth="1"/>
-    <col min="39" max="39" width="23" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="2"/>
+    <col min="9" max="9" width="22.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="38" width="9.109375" style="3" customWidth="1"/>
+    <col min="39" max="39" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.77734375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="23"/>
       <c r="I1" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="J1" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
-      <c r="AK1" s="18"/>
-      <c r="AL1" s="19"/>
+      <c r="J1" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22"/>
+      <c r="AK1" s="22"/>
+      <c r="AL1" s="23"/>
       <c r="AM1" s="4" t="s">
         <v>241</v>
       </c>
@@ -1813,7 +1807,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1872,7 +1866,7 @@
       </c>
       <c r="AP2" s="3"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1904,7 +1898,7 @@
       </c>
       <c r="AP3" s="3"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1930,7 +1924,7 @@
       </c>
       <c r="AP4" s="3"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1956,7 +1950,7 @@
       </c>
       <c r="AP5" s="3"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1982,7 +1976,7 @@
       </c>
       <c r="AP6" s="3"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -2011,7 +2005,7 @@
       </c>
       <c r="AP7" s="7"/>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -2040,7 +2034,7 @@
       </c>
       <c r="AP8" s="3"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -2069,7 +2063,7 @@
       </c>
       <c r="AP9" s="3"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2095,7 +2089,7 @@
       </c>
       <c r="AP10" s="3"/>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -2121,7 +2115,7 @@
       </c>
       <c r="AP11" s="3"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -2159,7 +2153,7 @@
       </c>
       <c r="AP12" s="3"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -2188,7 +2182,7 @@
       </c>
       <c r="AP13" s="3"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -2215,14 +2209,14 @@
         <f t="shared" si="1"/>
         <v>repeat</v>
       </c>
-      <c r="AP14" s="20" t="s">
+      <c r="AP14" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="AQ14" s="20"/>
-      <c r="AR14" s="20"/>
-      <c r="AS14" s="20"/>
-    </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AQ14" s="24"/>
+      <c r="AR14" s="24"/>
+      <c r="AS14" s="24"/>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -2248,7 +2242,7 @@
       </c>
       <c r="AP15" s="3"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -2274,7 +2268,7 @@
       </c>
       <c r="AP16" s="3"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -2300,7 +2294,7 @@
       </c>
       <c r="AP17" s="3"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -2332,7 +2326,7 @@
       </c>
       <c r="AP18" s="3"/>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2361,7 +2355,7 @@
       </c>
       <c r="AP19" s="3"/>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -2387,7 +2381,7 @@
       </c>
       <c r="AP20" s="3"/>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -2419,7 +2413,7 @@
       </c>
       <c r="AP21" s="3"/>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -2457,7 +2451,7 @@
       </c>
       <c r="AP22" s="3"/>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -2483,7 +2477,7 @@
       </c>
       <c r="AP23" s="3"/>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -2512,7 +2506,7 @@
       </c>
       <c r="AP24" s="3"/>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -2544,7 +2538,7 @@
       </c>
       <c r="AP25" s="3"/>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -2570,7 +2564,7 @@
       </c>
       <c r="AP26" s="3"/>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
@@ -2596,7 +2590,7 @@
       </c>
       <c r="AP27" s="3"/>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -2631,7 +2625,7 @@
       </c>
       <c r="AP28" s="3"/>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -2743,7 +2737,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
@@ -2773,14 +2767,14 @@
         <f t="shared" si="1"/>
         <v>skip</v>
       </c>
-      <c r="AP30" s="20" t="s">
+      <c r="AP30" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="AQ30" s="20"/>
-      <c r="AR30" s="20"/>
-      <c r="AS30" s="20"/>
-    </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AQ30" s="24"/>
+      <c r="AR30" s="24"/>
+      <c r="AS30" s="24"/>
+    </row>
+    <row r="31" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
@@ -2811,7 +2805,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -2841,14 +2835,14 @@
         <f t="shared" si="1"/>
         <v>skip</v>
       </c>
-      <c r="AP32" s="12" t="s">
+      <c r="AP32" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="AQ32" s="12"/>
-      <c r="AR32" s="12"/>
-      <c r="AS32" s="12"/>
-    </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AQ32" s="13"/>
+      <c r="AR32" s="13"/>
+      <c r="AS32" s="13"/>
+    </row>
+    <row r="33" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
@@ -2882,7 +2876,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -2913,7 +2907,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -2938,7 +2932,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -2963,7 +2957,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -3012,7 +3006,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
@@ -3037,7 +3031,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="39" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
@@ -3062,7 +3056,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="40" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
@@ -3099,7 +3093,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="41" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
@@ -3127,7 +3121,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="42" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
@@ -3152,7 +3146,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
@@ -3180,7 +3174,7 @@
       <c r="AQ43" s="8"/>
       <c r="AR43" s="8"/>
     </row>
-    <row r="44" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
@@ -3211,7 +3205,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="45" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
@@ -3248,7 +3242,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="46" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
@@ -3276,7 +3270,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="47" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
@@ -3301,7 +3295,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="48" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>250</v>
       </c>
@@ -3326,7 +3320,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>46</v>
       </c>
@@ -3351,7 +3345,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>47</v>
       </c>
@@ -3382,7 +3376,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>48</v>
       </c>
@@ -3407,7 +3401,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>49</v>
       </c>
@@ -3432,7 +3426,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>50</v>
       </c>
@@ -3460,7 +3454,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>51</v>
       </c>
@@ -3497,7 +3491,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="55" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>52</v>
       </c>
@@ -3525,7 +3519,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="56" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>53</v>
       </c>
@@ -3553,7 +3547,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="57" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>54</v>
       </c>
@@ -3578,7 +3572,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="58" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>55</v>
       </c>
@@ -3606,7 +3600,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="59" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>56</v>
       </c>
@@ -3637,7 +3631,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="60" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>57</v>
       </c>
@@ -3683,7 +3677,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="61" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>58</v>
       </c>
@@ -3708,7 +3702,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="62" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>59</v>
       </c>
@@ -3751,7 +3745,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="63" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>60</v>
       </c>
@@ -3797,7 +3791,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="64" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>61</v>
       </c>
@@ -3825,7 +3819,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="65" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>62</v>
       </c>
@@ -3862,7 +3856,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="66" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>63</v>
       </c>
@@ -3887,17 +3881,17 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="67" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A67" s="21" t="s">
+    <row r="67" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A67" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B67" s="22">
+      <c r="B67" s="16">
         <v>493</v>
       </c>
-      <c r="C67" s="23">
+      <c r="C67" s="17">
         <v>5289</v>
       </c>
-      <c r="I67" s="13">
+      <c r="I67" s="14">
         <v>34.58</v>
       </c>
       <c r="J67">
@@ -3987,30 +3981,30 @@
       <c r="AL67" s="6">
         <v>13112</v>
       </c>
-      <c r="AM67" s="13">
+      <c r="AM67" s="14">
         <v>1983.03</v>
       </c>
-      <c r="AN67" s="13">
+      <c r="AN67" s="14">
         <f t="shared" si="2"/>
         <v>57.346153846153847</v>
       </c>
-      <c r="AO67" s="14" t="str">
+      <c r="AO67" s="19" t="str">
         <f t="shared" ref="AO67:AO134" si="3">IF(AN67&lt;2,"skip", "repeat")</f>
         <v>repeat</v>
       </c>
-      <c r="AP67" s="15" t="s">
+      <c r="AP67" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="AQ67" s="15"/>
-      <c r="AR67" s="15"/>
-      <c r="AS67" s="15"/>
+      <c r="AQ67" s="20"/>
+      <c r="AR67" s="20"/>
+      <c r="AS67" s="20"/>
       <c r="AT67" s="8"/>
     </row>
-    <row r="68" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A68" s="21"/>
-      <c r="B68" s="22"/>
-      <c r="C68" s="23"/>
-      <c r="I68" s="13"/>
+    <row r="68" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A68" s="15"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="17"/>
+      <c r="I68" s="14"/>
       <c r="J68">
         <v>13113</v>
       </c>
@@ -4098,20 +4092,20 @@
       <c r="AL68" s="6">
         <v>16437</v>
       </c>
-      <c r="AM68" s="13"/>
-      <c r="AN68" s="13"/>
-      <c r="AO68" s="14"/>
-      <c r="AP68" s="15"/>
-      <c r="AQ68" s="15"/>
-      <c r="AR68" s="15"/>
-      <c r="AS68" s="15"/>
+      <c r="AM68" s="14"/>
+      <c r="AN68" s="14"/>
+      <c r="AO68" s="19"/>
+      <c r="AP68" s="20"/>
+      <c r="AQ68" s="20"/>
+      <c r="AR68" s="20"/>
+      <c r="AS68" s="20"/>
       <c r="AT68" s="8"/>
     </row>
-    <row r="69" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A69" s="21"/>
-      <c r="B69" s="22"/>
-      <c r="C69" s="23"/>
-      <c r="I69" s="13"/>
+    <row r="69" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A69" s="15"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="17"/>
+      <c r="I69" s="14"/>
       <c r="J69">
         <v>16438</v>
       </c>
@@ -4199,20 +4193,20 @@
       <c r="AL69" s="6">
         <v>17686</v>
       </c>
-      <c r="AM69" s="13"/>
-      <c r="AN69" s="13"/>
-      <c r="AO69" s="14"/>
-      <c r="AP69" s="15"/>
-      <c r="AQ69" s="15"/>
-      <c r="AR69" s="15"/>
-      <c r="AS69" s="15"/>
+      <c r="AM69" s="14"/>
+      <c r="AN69" s="14"/>
+      <c r="AO69" s="19"/>
+      <c r="AP69" s="20"/>
+      <c r="AQ69" s="20"/>
+      <c r="AR69" s="20"/>
+      <c r="AS69" s="20"/>
       <c r="AT69" s="8"/>
     </row>
-    <row r="70" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A70" s="21"/>
-      <c r="B70" s="22"/>
-      <c r="C70" s="23"/>
-      <c r="I70" s="13"/>
+    <row r="70" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A70" s="15"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="17"/>
+      <c r="I70" s="14"/>
       <c r="J70">
         <v>18423</v>
       </c>
@@ -4300,20 +4294,20 @@
       <c r="AL70" s="6">
         <v>19879</v>
       </c>
-      <c r="AM70" s="13"/>
-      <c r="AN70" s="13"/>
-      <c r="AO70" s="14"/>
-      <c r="AP70" s="15"/>
-      <c r="AQ70" s="15"/>
-      <c r="AR70" s="15"/>
-      <c r="AS70" s="15"/>
+      <c r="AM70" s="14"/>
+      <c r="AN70" s="14"/>
+      <c r="AO70" s="19"/>
+      <c r="AP70" s="20"/>
+      <c r="AQ70" s="20"/>
+      <c r="AR70" s="20"/>
+      <c r="AS70" s="20"/>
       <c r="AT70" s="8"/>
     </row>
-    <row r="71" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A71" s="21"/>
-      <c r="B71" s="22"/>
-      <c r="C71" s="23"/>
-      <c r="I71" s="13"/>
+    <row r="71" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A71" s="15"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="17"/>
+      <c r="I71" s="14"/>
       <c r="J71">
         <v>19880</v>
       </c>
@@ -4371,16 +4365,16 @@
       <c r="AJ71" s="6"/>
       <c r="AK71" s="6"/>
       <c r="AL71" s="6"/>
-      <c r="AM71" s="13"/>
-      <c r="AN71" s="13"/>
-      <c r="AO71" s="14"/>
-      <c r="AP71" s="15"/>
-      <c r="AQ71" s="15"/>
-      <c r="AR71" s="15"/>
-      <c r="AS71" s="15"/>
+      <c r="AM71" s="14"/>
+      <c r="AN71" s="14"/>
+      <c r="AO71" s="19"/>
+      <c r="AP71" s="20"/>
+      <c r="AQ71" s="20"/>
+      <c r="AR71" s="20"/>
+      <c r="AS71" s="20"/>
       <c r="AT71" s="8"/>
     </row>
-    <row r="72" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>65</v>
       </c>
@@ -4417,14 +4411,14 @@
         <f t="shared" si="3"/>
         <v>repeat</v>
       </c>
-      <c r="AP72" s="12" t="s">
-        <v>269</v>
-      </c>
-      <c r="AQ72" s="12"/>
-      <c r="AR72" s="12"/>
-      <c r="AS72" s="12"/>
-    </row>
-    <row r="73" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AP72" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="AQ72" s="13"/>
+      <c r="AR72" s="13"/>
+      <c r="AS72" s="13"/>
+    </row>
+    <row r="73" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>66</v>
       </c>
@@ -4467,7 +4461,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="74" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>67</v>
       </c>
@@ -4495,7 +4489,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="75" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>68</v>
       </c>
@@ -4520,7 +4514,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="76" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>69</v>
       </c>
@@ -4551,7 +4545,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="77" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>70</v>
       </c>
@@ -4588,7 +4582,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="78" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>71</v>
       </c>
@@ -4628,7 +4622,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="79" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>72</v>
       </c>
@@ -4686,7 +4680,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="80" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>73</v>
       </c>
@@ -4723,7 +4717,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="81" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>74</v>
       </c>
@@ -4751,7 +4745,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="82" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>75</v>
       </c>
@@ -4776,7 +4770,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="83" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>76</v>
       </c>
@@ -4801,7 +4795,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="84" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>77</v>
       </c>
@@ -4826,7 +4820,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="85" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>78</v>
       </c>
@@ -4854,7 +4848,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="86" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>79</v>
       </c>
@@ -4879,7 +4873,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="87" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>80</v>
       </c>
@@ -4907,7 +4901,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="88" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>81</v>
       </c>
@@ -4956,7 +4950,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="89" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>82</v>
       </c>
@@ -4981,7 +4975,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="90" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>83</v>
       </c>
@@ -5021,7 +5015,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="91" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>84</v>
       </c>
@@ -5049,7 +5043,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="92" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>85</v>
       </c>
@@ -5074,7 +5068,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="93" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>86</v>
       </c>
@@ -5114,7 +5108,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="94" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>87</v>
       </c>
@@ -5151,7 +5145,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="95" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>88</v>
       </c>
@@ -5185,7 +5179,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="96" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>89</v>
       </c>
@@ -5228,7 +5222,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="97" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>90</v>
       </c>
@@ -5256,7 +5250,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="98" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>91</v>
       </c>
@@ -5284,7 +5278,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="99" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>92</v>
       </c>
@@ -5330,7 +5324,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="100" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>93</v>
       </c>
@@ -5355,7 +5349,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="101" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>94</v>
       </c>
@@ -5383,7 +5377,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="102" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>95</v>
       </c>
@@ -5411,7 +5405,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="103" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>96</v>
       </c>
@@ -5439,7 +5433,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="104" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>97</v>
       </c>
@@ -5464,7 +5458,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="105" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>98</v>
       </c>
@@ -5495,7 +5489,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="106" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>99</v>
       </c>
@@ -5520,7 +5514,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="107" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>100</v>
       </c>
@@ -5545,7 +5539,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="108" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>101</v>
       </c>
@@ -5570,7 +5564,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="109" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>102</v>
       </c>
@@ -5598,7 +5592,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="110" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>103</v>
       </c>
@@ -5623,7 +5617,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="111" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>104</v>
       </c>
@@ -5648,7 +5642,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="112" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>105</v>
       </c>
@@ -5682,7 +5676,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="113" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>106</v>
       </c>
@@ -5701,25 +5695,56 @@
       <c r="L113">
         <v>7329</v>
       </c>
+      <c r="M113">
+        <v>19596</v>
+      </c>
+      <c r="N113">
+        <v>19597</v>
+      </c>
+      <c r="O113">
+        <v>19598</v>
+      </c>
+      <c r="P113">
+        <v>20626</v>
+      </c>
+      <c r="Q113">
+        <v>20627</v>
+      </c>
+      <c r="R113">
+        <v>20628</v>
+      </c>
+      <c r="S113">
+        <v>20629</v>
+      </c>
+      <c r="T113" s="3">
+        <v>20805</v>
+      </c>
+      <c r="U113" s="6">
+        <v>20806</v>
+      </c>
+      <c r="V113" s="6">
+        <v>20811</v>
+      </c>
+      <c r="W113" s="6">
+        <v>20817</v>
+      </c>
       <c r="AM113" s="4">
-        <v>151.63999999999999</v>
+        <v>625.91</v>
       </c>
       <c r="AN113" s="4">
         <f t="shared" si="2"/>
-        <v>3.853621346886912</v>
+        <v>15.906226175349428</v>
       </c>
       <c r="AO113" t="str">
         <f t="shared" si="3"/>
         <v>repeat</v>
       </c>
-      <c r="AP113" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="AQ113" s="16"/>
-      <c r="AR113" s="16"/>
-      <c r="AS113" s="16"/>
-    </row>
-    <row r="114" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP113" s="8"/>
+      <c r="AQ113" s="8"/>
+      <c r="AR113" s="8"/>
+      <c r="AS113" s="8"/>
+    </row>
+    <row r="114" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>107</v>
       </c>
@@ -5746,12 +5771,12 @@
         <f t="shared" si="3"/>
         <v>repeat</v>
       </c>
-      <c r="AP114" s="16"/>
-      <c r="AQ114" s="16"/>
-      <c r="AR114" s="16"/>
-      <c r="AS114" s="16"/>
-    </row>
-    <row r="115" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP114" s="8"/>
+      <c r="AQ114" s="8"/>
+      <c r="AR114" s="8"/>
+      <c r="AS114" s="8"/>
+    </row>
+    <row r="115" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>108</v>
       </c>
@@ -5778,12 +5803,12 @@
         <f t="shared" si="3"/>
         <v>repeat</v>
       </c>
-      <c r="AP115" s="16"/>
-      <c r="AQ115" s="16"/>
-      <c r="AR115" s="16"/>
-      <c r="AS115" s="16"/>
-    </row>
-    <row r="116" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP115" s="8"/>
+      <c r="AQ115" s="8"/>
+      <c r="AR115" s="8"/>
+      <c r="AS115" s="8"/>
+    </row>
+    <row r="116" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>109</v>
       </c>
@@ -5808,7 +5833,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="117" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>110</v>
       </c>
@@ -5833,7 +5858,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="118" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>111</v>
       </c>
@@ -5857,14 +5882,14 @@
         <f t="shared" si="3"/>
         <v>skip</v>
       </c>
-      <c r="AP118" s="12" t="s">
-        <v>264</v>
-      </c>
-      <c r="AQ118" s="12"/>
-      <c r="AR118" s="12"/>
-      <c r="AS118" s="12"/>
-    </row>
-    <row r="119" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP118" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="AQ118" s="13"/>
+      <c r="AR118" s="13"/>
+      <c r="AS118" s="13"/>
+    </row>
+    <row r="119" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>112</v>
       </c>
@@ -5910,7 +5935,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="120" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>113</v>
       </c>
@@ -5956,7 +5981,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="121" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>114</v>
       </c>
@@ -5981,7 +6006,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="122" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>115</v>
       </c>
@@ -6006,7 +6031,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="123" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>116</v>
       </c>
@@ -6036,14 +6061,14 @@
         <f t="shared" si="3"/>
         <v>repeat</v>
       </c>
-      <c r="AP123" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="AQ123" s="12"/>
-      <c r="AR123" s="12"/>
-      <c r="AS123" s="12"/>
-    </row>
-    <row r="124" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP123" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="AQ123" s="13"/>
+      <c r="AR123" s="13"/>
+      <c r="AS123" s="13"/>
+    </row>
+    <row r="124" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>117</v>
       </c>
@@ -6068,7 +6093,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="125" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>118</v>
       </c>
@@ -6102,7 +6127,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="126" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>119</v>
       </c>
@@ -6130,7 +6155,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="127" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>120</v>
       </c>
@@ -6155,7 +6180,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="128" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>121</v>
       </c>
@@ -6186,7 +6211,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="129" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>122</v>
       </c>
@@ -6211,7 +6236,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="130" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>123</v>
       </c>
@@ -6239,7 +6264,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="131" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>124</v>
       </c>
@@ -6264,7 +6289,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="132" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>125</v>
       </c>
@@ -6289,7 +6314,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="133" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>126</v>
       </c>
@@ -6314,7 +6339,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="134" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>127</v>
       </c>
@@ -6339,7 +6364,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="135" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>128</v>
       </c>
@@ -6367,7 +6392,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="136" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>129</v>
       </c>
@@ -6425,7 +6450,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="137" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>130</v>
       </c>
@@ -6450,7 +6475,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="138" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>131</v>
       </c>
@@ -6475,7 +6500,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="139" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>132</v>
       </c>
@@ -6500,7 +6525,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="140" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>133</v>
       </c>
@@ -6528,7 +6553,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="141" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>134</v>
       </c>
@@ -6556,7 +6581,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="142" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>135</v>
       </c>
@@ -6584,7 +6609,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="143" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>136</v>
       </c>
@@ -6618,7 +6643,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="144" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>137</v>
       </c>
@@ -6643,7 +6668,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="145" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>138</v>
       </c>
@@ -6680,7 +6705,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="146" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>139</v>
       </c>
@@ -6765,7 +6790,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="147" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>140</v>
       </c>
@@ -6808,7 +6833,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="148" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>141</v>
       </c>
@@ -6845,14 +6870,14 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="149" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A149" s="21" t="s">
+    <row r="149" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A149" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="B149" s="22">
+      <c r="B149" s="16">
         <v>360</v>
       </c>
-      <c r="I149" s="13">
+      <c r="I149" s="14">
         <v>34.72</v>
       </c>
       <c r="J149" s="6">
@@ -6942,23 +6967,23 @@
       <c r="AL149" s="6">
         <v>17510</v>
       </c>
-      <c r="AM149" s="13">
+      <c r="AM149" s="14">
         <v>2116.58</v>
       </c>
-      <c r="AN149" s="25">
+      <c r="AN149" s="18">
         <f t="shared" si="4"/>
         <v>60.961405529953915</v>
       </c>
-      <c r="AO149" s="14" t="str">
+      <c r="AO149" s="19" t="str">
         <f t="shared" si="5"/>
         <v>repeat</v>
       </c>
       <c r="AT149" s="8"/>
     </row>
-    <row r="150" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A150" s="21"/>
-      <c r="B150" s="22"/>
-      <c r="I150" s="13"/>
+    <row r="150" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A150" s="15"/>
+      <c r="B150" s="16"/>
+      <c r="I150" s="14"/>
       <c r="J150" s="6">
         <v>17511</v>
       </c>
@@ -7046,15 +7071,15 @@
       <c r="AL150" s="6">
         <v>18886</v>
       </c>
-      <c r="AM150" s="13"/>
-      <c r="AN150" s="25"/>
-      <c r="AO150" s="14"/>
+      <c r="AM150" s="14"/>
+      <c r="AN150" s="18"/>
+      <c r="AO150" s="19"/>
       <c r="AT150" s="8"/>
     </row>
-    <row r="151" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A151" s="21"/>
-      <c r="B151" s="22"/>
-      <c r="I151" s="13"/>
+    <row r="151" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A151" s="15"/>
+      <c r="B151" s="16"/>
+      <c r="I151" s="14"/>
       <c r="J151" s="6">
         <v>19888</v>
       </c>
@@ -7106,12 +7131,12 @@
       <c r="AJ151" s="6"/>
       <c r="AK151" s="6"/>
       <c r="AL151" s="6"/>
-      <c r="AM151" s="13"/>
-      <c r="AN151" s="25"/>
-      <c r="AO151" s="14"/>
+      <c r="AM151" s="14"/>
+      <c r="AN151" s="18"/>
+      <c r="AO151" s="19"/>
       <c r="AT151" s="8"/>
     </row>
-    <row r="152" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>143</v>
       </c>
@@ -7142,7 +7167,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="153" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>144</v>
       </c>
@@ -7167,7 +7192,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="154" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>145</v>
       </c>
@@ -7192,7 +7217,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="155" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>146</v>
       </c>
@@ -7223,7 +7248,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="156" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>147</v>
       </c>
@@ -7248,7 +7273,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="157" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>148</v>
       </c>
@@ -7285,7 +7310,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="158" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>149</v>
       </c>
@@ -7299,10 +7324,10 @@
         <v>118.34</v>
       </c>
       <c r="J158" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K158" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L158">
         <v>4969</v>
@@ -7325,14 +7350,14 @@
         <f t="shared" si="5"/>
         <v>repeat</v>
       </c>
-      <c r="AP158" s="12" t="s">
-        <v>270</v>
-      </c>
-      <c r="AQ158" s="12"/>
-      <c r="AR158" s="12"/>
-      <c r="AS158" s="12"/>
-    </row>
-    <row r="159" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AP158" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="AQ158" s="13"/>
+      <c r="AR158" s="13"/>
+      <c r="AS158" s="13"/>
+    </row>
+    <row r="159" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>150</v>
       </c>
@@ -7369,17 +7394,17 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="160" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A160" s="21" t="s">
+    <row r="160" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A160" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="B160" s="22">
+      <c r="B160" s="16">
         <v>5826</v>
       </c>
-      <c r="C160" s="23">
+      <c r="C160" s="17">
         <v>5827</v>
       </c>
-      <c r="I160" s="13">
+      <c r="I160" s="14">
         <v>282.95999999999998</v>
       </c>
       <c r="J160">
@@ -7469,30 +7494,30 @@
       <c r="AL160" s="6">
         <v>5740</v>
       </c>
-      <c r="AM160" s="13">
+      <c r="AM160" s="14">
         <v>1438.31</v>
       </c>
-      <c r="AN160" s="13">
+      <c r="AN160" s="14">
         <f t="shared" si="4"/>
         <v>5.0830859485439639</v>
       </c>
-      <c r="AO160" s="14" t="str">
+      <c r="AO160" s="19" t="str">
         <f t="shared" si="5"/>
         <v>repeat</v>
       </c>
-      <c r="AP160" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="AQ160" s="15"/>
-      <c r="AR160" s="15"/>
-      <c r="AS160" s="15"/>
+      <c r="AP160" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="AQ160" s="20"/>
+      <c r="AR160" s="20"/>
+      <c r="AS160" s="20"/>
       <c r="AT160" s="8"/>
     </row>
-    <row r="161" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A161" s="21"/>
-      <c r="B161" s="22"/>
-      <c r="C161" s="23"/>
-      <c r="I161" s="13"/>
+    <row r="161" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A161" s="15"/>
+      <c r="B161" s="16"/>
+      <c r="C161" s="17"/>
+      <c r="I161" s="14"/>
       <c r="J161">
         <v>5741</v>
       </c>
@@ -7580,20 +7605,20 @@
       <c r="AL161" s="5">
         <v>7351</v>
       </c>
-      <c r="AM161" s="13"/>
-      <c r="AN161" s="13"/>
-      <c r="AO161" s="14"/>
-      <c r="AP161" s="15"/>
-      <c r="AQ161" s="15"/>
-      <c r="AR161" s="15"/>
-      <c r="AS161" s="15"/>
+      <c r="AM161" s="14"/>
+      <c r="AN161" s="14"/>
+      <c r="AO161" s="19"/>
+      <c r="AP161" s="20"/>
+      <c r="AQ161" s="20"/>
+      <c r="AR161" s="20"/>
+      <c r="AS161" s="20"/>
       <c r="AT161" s="8"/>
     </row>
-    <row r="162" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A162" s="21"/>
-      <c r="B162" s="22"/>
-      <c r="C162" s="23"/>
-      <c r="I162" s="13"/>
+    <row r="162" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A162" s="15"/>
+      <c r="B162" s="16"/>
+      <c r="C162" s="17"/>
+      <c r="I162" s="14"/>
       <c r="J162">
         <v>7352</v>
       </c>
@@ -7681,20 +7706,20 @@
       <c r="AL162" s="6">
         <v>11515</v>
       </c>
-      <c r="AM162" s="13"/>
-      <c r="AN162" s="13"/>
-      <c r="AO162" s="14"/>
-      <c r="AP162" s="15"/>
-      <c r="AQ162" s="15"/>
-      <c r="AR162" s="15"/>
-      <c r="AS162" s="15"/>
+      <c r="AM162" s="14"/>
+      <c r="AN162" s="14"/>
+      <c r="AO162" s="19"/>
+      <c r="AP162" s="20"/>
+      <c r="AQ162" s="20"/>
+      <c r="AR162" s="20"/>
+      <c r="AS162" s="20"/>
       <c r="AT162" s="8"/>
     </row>
-    <row r="163" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A163" s="21"/>
-      <c r="B163" s="22"/>
-      <c r="C163" s="23"/>
-      <c r="I163" s="13"/>
+    <row r="163" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A163" s="15"/>
+      <c r="B163" s="16"/>
+      <c r="C163" s="17"/>
+      <c r="I163" s="14"/>
       <c r="J163">
         <v>11516</v>
       </c>
@@ -7782,20 +7807,20 @@
       <c r="AL163" s="5">
         <v>19458</v>
       </c>
-      <c r="AM163" s="13"/>
-      <c r="AN163" s="13"/>
-      <c r="AO163" s="14"/>
-      <c r="AP163" s="15"/>
-      <c r="AQ163" s="15"/>
-      <c r="AR163" s="15"/>
-      <c r="AS163" s="15"/>
+      <c r="AM163" s="14"/>
+      <c r="AN163" s="14"/>
+      <c r="AO163" s="19"/>
+      <c r="AP163" s="20"/>
+      <c r="AQ163" s="20"/>
+      <c r="AR163" s="20"/>
+      <c r="AS163" s="20"/>
       <c r="AT163" s="8"/>
     </row>
-    <row r="164" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A164" s="21"/>
-      <c r="B164" s="22"/>
-      <c r="C164" s="23"/>
-      <c r="I164" s="13"/>
+    <row r="164" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A164" s="15"/>
+      <c r="B164" s="16"/>
+      <c r="C164" s="17"/>
+      <c r="I164" s="14"/>
       <c r="J164">
         <v>20034</v>
       </c>
@@ -7808,16 +7833,16 @@
       <c r="M164" s="6">
         <v>21076</v>
       </c>
-      <c r="AM164" s="13"/>
-      <c r="AN164" s="13"/>
-      <c r="AO164" s="14"/>
-      <c r="AP164" s="15"/>
-      <c r="AQ164" s="15"/>
-      <c r="AR164" s="15"/>
-      <c r="AS164" s="15"/>
+      <c r="AM164" s="14"/>
+      <c r="AN164" s="14"/>
+      <c r="AO164" s="19"/>
+      <c r="AP164" s="20"/>
+      <c r="AQ164" s="20"/>
+      <c r="AR164" s="20"/>
+      <c r="AS164" s="20"/>
       <c r="AT164" s="8"/>
     </row>
-    <row r="165" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>152</v>
       </c>
@@ -7848,7 +7873,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="166" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>153</v>
       </c>
@@ -7873,7 +7898,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="167" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>154</v>
       </c>
@@ -7907,7 +7932,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="168" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>155</v>
       </c>
@@ -7932,7 +7957,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="169" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>156</v>
       </c>
@@ -7963,7 +7988,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="170" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>157</v>
       </c>
@@ -7988,7 +8013,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="171" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>158</v>
       </c>
@@ -8013,7 +8038,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="172" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>159</v>
       </c>
@@ -8053,7 +8078,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="173" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>160</v>
       </c>
@@ -8084,7 +8109,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="174" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>161</v>
       </c>
@@ -8109,7 +8134,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="175" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>162</v>
       </c>
@@ -8134,7 +8159,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="176" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>163</v>
       </c>
@@ -8159,7 +8184,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="177" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>164</v>
       </c>
@@ -8196,7 +8221,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="178" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>165</v>
       </c>
@@ -8233,7 +8258,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="179" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>166</v>
       </c>
@@ -8270,7 +8295,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="180" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>167</v>
       </c>
@@ -8301,7 +8326,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="181" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>168</v>
       </c>
@@ -8329,7 +8354,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="182" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>169</v>
       </c>
@@ -8378,7 +8403,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="183" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>170</v>
       </c>
@@ -8403,7 +8428,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="184" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>171</v>
       </c>
@@ -8440,7 +8465,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="185" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>172</v>
       </c>
@@ -8492,7 +8517,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="186" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>173</v>
       </c>
@@ -8520,7 +8545,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="187" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>174</v>
       </c>
@@ -8545,7 +8570,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="188" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>175</v>
       </c>
@@ -8570,7 +8595,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="189" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>176</v>
       </c>
@@ -8601,9 +8626,9 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="190" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B190">
         <v>3285</v>
@@ -8626,7 +8651,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="191" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>177</v>
       </c>
@@ -8654,7 +8679,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="192" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>178</v>
       </c>
@@ -8679,7 +8704,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="193" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>179</v>
       </c>
@@ -8704,7 +8729,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="194" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>180</v>
       </c>
@@ -8729,7 +8754,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="195" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>181</v>
       </c>
@@ -8760,9 +8785,9 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="196" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B196">
         <v>520</v>
@@ -8785,7 +8810,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="197" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>182</v>
       </c>
@@ -8810,7 +8835,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="198" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>183</v>
       </c>
@@ -8835,7 +8860,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="199" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>184</v>
       </c>
@@ -8863,7 +8888,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="200" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>185</v>
       </c>
@@ -8912,7 +8937,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="201" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>186</v>
       </c>
@@ -8940,7 +8965,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="202" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
         <v>187</v>
       </c>
@@ -8968,7 +8993,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="203" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
         <v>188</v>
       </c>
@@ -8996,7 +9021,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="204" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
         <v>189</v>
       </c>
@@ -9024,7 +9049,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="205" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>190</v>
       </c>
@@ -9055,7 +9080,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="206" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>191</v>
       </c>
@@ -9086,7 +9111,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="207" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
         <v>192</v>
       </c>
@@ -9114,7 +9139,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="208" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>193</v>
       </c>
@@ -9142,7 +9167,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="209" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>194</v>
       </c>
@@ -9179,7 +9204,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="210" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>195</v>
       </c>
@@ -9224,14 +9249,14 @@
         <f t="shared" si="7"/>
         <v>repeat</v>
       </c>
-      <c r="AP210" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="AQ210" s="12"/>
-      <c r="AR210" s="12"/>
-      <c r="AS210" s="12"/>
-    </row>
-    <row r="211" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP210" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="AQ210" s="13"/>
+      <c r="AR210" s="13"/>
+      <c r="AS210" s="13"/>
+    </row>
+    <row r="211" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>196</v>
       </c>
@@ -9280,7 +9305,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="212" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>197</v>
       </c>
@@ -9311,7 +9336,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="213" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>198</v>
       </c>
@@ -9363,7 +9388,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="214" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>199</v>
       </c>
@@ -9405,14 +9430,14 @@
         <f t="shared" si="7"/>
         <v>repeat</v>
       </c>
-      <c r="AP214" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="AQ214" s="12"/>
-      <c r="AR214" s="12"/>
-      <c r="AS214" s="12"/>
-    </row>
-    <row r="215" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP214" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="AQ214" s="13"/>
+      <c r="AR214" s="13"/>
+      <c r="AS214" s="13"/>
+    </row>
+    <row r="215" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>200</v>
       </c>
@@ -9437,7 +9462,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="216" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>201</v>
       </c>
@@ -9480,7 +9505,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="217" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>202</v>
       </c>
@@ -9511,7 +9536,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="218" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>203</v>
       </c>
@@ -9542,7 +9567,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="219" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>204</v>
       </c>
@@ -9573,7 +9598,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="220" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>205</v>
       </c>
@@ -9598,7 +9623,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="221" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
         <v>206</v>
       </c>
@@ -9623,7 +9648,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="222" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>207</v>
       </c>
@@ -9648,7 +9673,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="223" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
         <v>208</v>
       </c>
@@ -9679,7 +9704,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="224" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
         <v>209</v>
       </c>
@@ -9716,7 +9741,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="225" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
         <v>210</v>
       </c>
@@ -9747,7 +9772,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="226" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>211</v>
       </c>
@@ -9778,7 +9803,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="227" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
         <v>212</v>
       </c>
@@ -9803,7 +9828,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="228" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
         <v>213</v>
       </c>
@@ -9828,7 +9853,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="229" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
         <v>214</v>
       </c>
@@ -9853,7 +9878,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="230" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
         <v>215</v>
       </c>
@@ -9878,7 +9903,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="231" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
         <v>216</v>
       </c>
@@ -9906,7 +9931,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="232" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
         <v>217</v>
       </c>
@@ -9948,14 +9973,14 @@
         <f t="shared" si="7"/>
         <v>repeat</v>
       </c>
-      <c r="AP232" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="AQ232" s="12"/>
-      <c r="AR232" s="12"/>
-      <c r="AS232" s="12"/>
-    </row>
-    <row r="233" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP232" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="AQ232" s="13"/>
+      <c r="AR232" s="13"/>
+      <c r="AS232" s="13"/>
+    </row>
+    <row r="233" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A233" s="2" t="s">
         <v>218</v>
       </c>
@@ -9986,7 +10011,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="234" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
         <v>219</v>
       </c>
@@ -10023,7 +10048,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="235" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
         <v>220</v>
       </c>
@@ -10057,7 +10082,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="236" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
         <v>221</v>
       </c>
@@ -10082,7 +10107,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="237" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
         <v>222</v>
       </c>
@@ -10119,7 +10144,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="238" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A238" s="2" t="s">
         <v>223</v>
       </c>
@@ -10159,7 +10184,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="239" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
         <v>224</v>
       </c>
@@ -10184,7 +10209,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="240" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
         <v>225</v>
       </c>
@@ -10212,7 +10237,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="241" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
         <v>226</v>
       </c>
@@ -10237,7 +10262,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="242" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
         <v>227</v>
       </c>
@@ -10265,7 +10290,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="243" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
         <v>228</v>
       </c>
@@ -10290,7 +10315,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="244" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
         <v>229</v>
       </c>
@@ -10315,7 +10340,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="245" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
         <v>230</v>
       </c>
@@ -10346,7 +10371,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="246" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
         <v>231</v>
       </c>
@@ -10371,7 +10396,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="247" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
         <v>232</v>
       </c>
@@ -10399,7 +10424,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="248" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
         <v>233</v>
       </c>
@@ -10427,7 +10452,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="249" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
         <v>234</v>
       </c>
@@ -10455,7 +10480,7 @@
         <v>skip</v>
       </c>
     </row>
-    <row r="250" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
         <v>235</v>
       </c>
@@ -10482,14 +10507,14 @@
         <f t="shared" si="7"/>
         <v>skip</v>
       </c>
-      <c r="AP250" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="AQ250" s="12"/>
-      <c r="AR250" s="12"/>
-      <c r="AS250" s="12"/>
-    </row>
-    <row r="251" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP250" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="AQ250" s="13"/>
+      <c r="AR250" s="13"/>
+      <c r="AS250" s="13"/>
+    </row>
+    <row r="251" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A251" s="2" t="s">
         <v>236</v>
       </c>
@@ -10520,7 +10545,7 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="252" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A252" s="2" t="s">
         <v>237</v>
       </c>
@@ -10548,53 +10573,75 @@
         <v>repeat</v>
       </c>
     </row>
-    <row r="254" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="B254" s="24" t="s">
         <v>260</v>
       </c>
-      <c r="C254" s="12"/>
-      <c r="D254" s="12"/>
+      <c r="B254" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="C254" s="13"/>
+      <c r="D254" s="13"/>
       <c r="I254" s="2">
         <f>SUM(I2:I252)</f>
         <v>10711.909999999994</v>
       </c>
-      <c r="J254" s="24" t="s">
-        <v>267</v>
-      </c>
-      <c r="K254" s="12"/>
-      <c r="L254" s="12"/>
+      <c r="J254" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="K254" s="13"/>
+      <c r="L254" s="13"/>
       <c r="AM254" s="4">
         <f>SUM(AM2:AM252)</f>
-        <v>28384.629999999983</v>
+        <v>28858.899999999987</v>
       </c>
       <c r="AN254" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="AO254" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="AO254" s="24" t="s">
-        <v>259</v>
-      </c>
-      <c r="AP254" s="12"/>
-    </row>
-    <row r="255" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP254" s="13"/>
+    </row>
+    <row r="255" spans="1:45" x14ac:dyDescent="0.3">
       <c r="I255" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="AM255" s="11" t="s">
         <v>262</v>
-      </c>
-      <c r="AM255" s="11" t="s">
-        <v>263</v>
       </c>
       <c r="AN255" s="4">
         <f>AVERAGE(AN2:AN252)</f>
-        <v>3.0214802848128071</v>
+        <v>3.071491093229664</v>
       </c>
       <c r="AO255">
         <v>77</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="39">
+  <mergeCells count="38">
+    <mergeCell ref="AP210:AS210"/>
+    <mergeCell ref="AP214:AS214"/>
+    <mergeCell ref="AP123:AS123"/>
+    <mergeCell ref="AN160:AN164"/>
+    <mergeCell ref="AO160:AO164"/>
+    <mergeCell ref="AP118:AS118"/>
+    <mergeCell ref="AP72:AS72"/>
+    <mergeCell ref="AP158:AS158"/>
+    <mergeCell ref="AP160:AS164"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="J1:AL1"/>
+    <mergeCell ref="AP30:AS30"/>
+    <mergeCell ref="AP14:AS14"/>
+    <mergeCell ref="AP32:AS32"/>
+    <mergeCell ref="AP67:AS71"/>
+    <mergeCell ref="AN67:AN71"/>
+    <mergeCell ref="AO67:AO71"/>
+    <mergeCell ref="A67:A71"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="C67:C71"/>
+    <mergeCell ref="I67:I71"/>
+    <mergeCell ref="AM67:AM71"/>
     <mergeCell ref="AO254:AP254"/>
     <mergeCell ref="J254:L254"/>
     <mergeCell ref="AM149:AM151"/>
@@ -10611,29 +10658,6 @@
     <mergeCell ref="AP250:AS250"/>
     <mergeCell ref="AN149:AN151"/>
     <mergeCell ref="AO149:AO151"/>
-    <mergeCell ref="A67:A71"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="C67:C71"/>
-    <mergeCell ref="I67:I71"/>
-    <mergeCell ref="AM67:AM71"/>
-    <mergeCell ref="AP118:AS118"/>
-    <mergeCell ref="AP72:AS72"/>
-    <mergeCell ref="AP158:AS158"/>
-    <mergeCell ref="AP160:AS164"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="J1:AL1"/>
-    <mergeCell ref="AP30:AS30"/>
-    <mergeCell ref="AP14:AS14"/>
-    <mergeCell ref="AP32:AS32"/>
-    <mergeCell ref="AP67:AS71"/>
-    <mergeCell ref="AN67:AN71"/>
-    <mergeCell ref="AO67:AO71"/>
-    <mergeCell ref="AP113:AS115"/>
-    <mergeCell ref="AP210:AS210"/>
-    <mergeCell ref="AP214:AS214"/>
-    <mergeCell ref="AP123:AS123"/>
-    <mergeCell ref="AN160:AN164"/>
-    <mergeCell ref="AO160:AO164"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>